<commit_message>
Baggage trains and significant restructuring of Vehicle class. Start op and End op are now lists for more flexibility, end goal has been removed and moved to normal goals for simplicity. All vehicles will need to be checked after this!
</commit_message>
<xml_diff>
--- a/assets/Meshes/Mesh_Water.xlsx
+++ b/assets/Meshes/Mesh_Water.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\assets\Meshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A970665-3F6F-4197-8186-2A83E176A38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD0D8C9-7CEE-4FCA-9284-AA7327A3BFC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,8 +343,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:GJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="CX39" sqref="CX39"/>
+    <sheetView tabSelected="1" topLeftCell="AO16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CA31" sqref="BO26:CA31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15003,43 +15003,43 @@
         <v>1</v>
       </c>
       <c r="BO26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB26" s="1">
         <v>1</v>
@@ -15581,43 +15581,43 @@
         <v>1</v>
       </c>
       <c r="BO27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB27" s="1">
         <v>1</v>
@@ -16159,43 +16159,43 @@
         <v>1</v>
       </c>
       <c r="BO28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB28" s="1">
         <v>1</v>
@@ -16737,43 +16737,43 @@
         <v>1</v>
       </c>
       <c r="BO29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB29" s="1">
         <v>1</v>
@@ -17315,43 +17315,43 @@
         <v>1</v>
       </c>
       <c r="BO30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB30" s="1">
         <v>1</v>
@@ -17836,100 +17836,100 @@
         <v>1</v>
       </c>
       <c r="AV31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB31" s="1">
         <v>1</v>
@@ -18414,100 +18414,100 @@
         <v>1</v>
       </c>
       <c r="AV32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB32" s="1">
         <v>1</v>
@@ -18992,100 +18992,100 @@
         <v>1</v>
       </c>
       <c r="AV33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB33" s="1">
         <v>1</v>
@@ -19570,100 +19570,100 @@
         <v>1</v>
       </c>
       <c r="AV34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB34" s="1">
         <v>1</v>
@@ -20148,100 +20148,100 @@
         <v>1</v>
       </c>
       <c r="AV35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB35" s="1">
         <v>1</v>
@@ -20726,100 +20726,100 @@
         <v>1</v>
       </c>
       <c r="AV36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB36" s="1">
         <v>1</v>
@@ -21304,100 +21304,100 @@
         <v>1</v>
       </c>
       <c r="AV37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB37" s="1">
         <v>1</v>
@@ -21882,100 +21882,100 @@
         <v>1</v>
       </c>
       <c r="AV38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB38" s="1">
         <v>1</v>
@@ -22460,100 +22460,100 @@
         <v>1</v>
       </c>
       <c r="AV39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB39" s="1">
         <v>1</v>
@@ -23038,124 +23038,124 @@
         <v>1</v>
       </c>
       <c r="AV40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ40" s="1">
         <v>0</v>
@@ -23616,124 +23616,124 @@
         <v>1</v>
       </c>
       <c r="AV41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ41" s="1">
         <v>0</v>
@@ -24194,124 +24194,124 @@
         <v>1</v>
       </c>
       <c r="AV42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ42" s="1">
         <v>0</v>
@@ -24772,124 +24772,124 @@
         <v>1</v>
       </c>
       <c r="AV43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ43" s="1">
         <v>0</v>
@@ -25350,124 +25350,124 @@
         <v>1</v>
       </c>
       <c r="AV44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ44" s="1">
         <v>0</v>
@@ -25928,124 +25928,124 @@
         <v>1</v>
       </c>
       <c r="AV45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ45" s="1">
         <v>0</v>
@@ -26506,124 +26506,124 @@
         <v>1</v>
       </c>
       <c r="AV46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ46" s="1">
         <v>0</v>
@@ -27084,124 +27084,124 @@
         <v>1</v>
       </c>
       <c r="AV47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ47" s="1">
         <v>0</v>
@@ -27662,124 +27662,124 @@
         <v>1</v>
       </c>
       <c r="AV48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ48" s="1">
         <v>0</v>
@@ -28240,124 +28240,124 @@
         <v>1</v>
       </c>
       <c r="AV49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ49" s="1">
         <v>0</v>
@@ -28818,124 +28818,124 @@
         <v>1</v>
       </c>
       <c r="AV50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ50" s="1">
         <v>0</v>
@@ -29396,124 +29396,124 @@
         <v>1</v>
       </c>
       <c r="AV51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ51" s="1">
         <v>0</v>
@@ -29974,124 +29974,124 @@
         <v>1</v>
       </c>
       <c r="AV52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BC52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ52" s="1">
         <v>0</v>
@@ -30579,97 +30579,97 @@
         <v>0</v>
       </c>
       <c r="BE53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ53" s="1">
         <v>0</v>
@@ -31160,94 +31160,94 @@
         <v>0</v>
       </c>
       <c r="BF54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ54" s="1">
         <v>0</v>
@@ -31738,94 +31738,94 @@
         <v>0</v>
       </c>
       <c r="BF55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BI55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ55" s="1">
         <v>0</v>
@@ -32325,85 +32325,85 @@
         <v>0</v>
       </c>
       <c r="BI56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BJ56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BK56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ56" s="1">
         <v>0</v>
@@ -32912,76 +32912,76 @@
         <v>0</v>
       </c>
       <c r="BL57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ57" s="1">
         <v>0</v>
@@ -33499,67 +33499,67 @@
         <v>0</v>
       </c>
       <c r="BO58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BQ58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ58" s="1">
         <v>0</v>
@@ -34086,58 +34086,58 @@
         <v>0</v>
       </c>
       <c r="BR59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ59" s="1">
         <v>0</v>
@@ -34673,49 +34673,49 @@
         <v>0</v>
       </c>
       <c r="BU60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ60" s="1">
         <v>0</v>
@@ -35260,40 +35260,40 @@
         <v>0</v>
       </c>
       <c r="BX61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ61" s="1">
         <v>0</v>
@@ -35847,31 +35847,31 @@
         <v>0</v>
       </c>
       <c r="CA62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ62" s="1">
         <v>0</v>
@@ -36437,19 +36437,19 @@
         <v>0</v>
       </c>
       <c r="CE63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ63" s="1">
         <v>0</v>
@@ -37027,7 +37027,7 @@
         <v>0</v>
       </c>
       <c r="CI64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ64" s="1">
         <v>0</v>

</xml_diff>